<commit_message>
Modified LIDO class for linking.
</commit_message>
<xml_diff>
--- a/aliada/aliada-links-discovery/src/main/resources/ALIADA_datasets_links.xlsx
+++ b/aliada/aliada-links-discovery/src/main/resources/ALIADA_datasets_links.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="19440" windowHeight="7170" activeTab="7"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="19440" windowHeight="7170"/>
   </bookViews>
   <sheets>
     <sheet name="DBpedia" sheetId="5" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="102">
   <si>
     <t>Actor</t>
   </si>
@@ -81,9 +81,6 @@
   </si>
   <si>
     <t>PREFIX ecrm:   &lt;http://erlangen-crm.org/current/&gt;</t>
-  </si>
-  <si>
-    <t>ecrm:E22_Man-Made_Object</t>
   </si>
   <si>
     <t xml:space="preserve"># Triples: 2.46 billion pieces of information (RDF triples) </t>
@@ -165,9 +162,6 @@
   </si>
   <si>
     <t>dbpediaprop:name</t>
-  </si>
-  <si>
-    <t>dbpediaprop:title</t>
   </si>
   <si>
     <t>PREFIX wgs84:   &lt;http://www.w3.org/2003/01/geo/wgs84_pos#&gt;</t>
@@ -330,6 +324,9 @@
   </si>
   <si>
     <t>graph: http://id.loc.gov/vocabulary/geographicAreas</t>
+  </si>
+  <si>
+    <t>ecrm:E19_Physical_Object</t>
   </si>
 </sst>
 </file>
@@ -900,8 +897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N535"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -922,17 +919,17 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -942,17 +939,17 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -1061,7 +1058,7 @@
         <v>0</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>6</v>
@@ -1076,17 +1073,17 @@
         <v>8</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L14" s="7"/>
       <c r="M14" s="4"/>
@@ -1097,7 +1094,7 @@
         <v>17</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>13</v>
@@ -1112,17 +1109,17 @@
         <v>8</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L15" s="7"/>
       <c r="M15" s="4"/>
@@ -1133,7 +1130,7 @@
         <v>12</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>20</v>
+        <v>101</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>15</v>
@@ -1148,17 +1145,17 @@
         <v>8</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H16" s="5"/>
       <c r="I16" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L16" s="7"/>
       <c r="M16" s="4"/>
@@ -1166,35 +1163,35 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C17" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D17" s="6" t="s">
-        <v>77</v>
-      </c>
       <c r="E17" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>8</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H17" s="5"/>
       <c r="I17" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L17" s="7"/>
       <c r="M17" s="4"/>
@@ -5765,17 +5762,17 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -5785,17 +5782,17 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -5809,7 +5806,7 @@
       <c r="F11" s="22"/>
       <c r="G11" s="23"/>
       <c r="I11" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J11" s="22"/>
       <c r="K11" s="22"/>
@@ -5887,13 +5884,13 @@
         <v>17</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="4"/>
@@ -5903,10 +5900,10 @@
         <v>18</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L14" s="7"/>
       <c r="M14" s="4"/>
@@ -5916,7 +5913,7 @@
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>13</v>
@@ -5931,17 +5928,17 @@
         <v>8</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="7" t="s">
         <v>18</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L15" s="7"/>
       <c r="M15" s="4"/>
@@ -13233,7 +13230,7 @@
   <dimension ref="A1:N543"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13251,17 +13248,17 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -13271,22 +13268,22 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -13301,7 +13298,7 @@
       <c r="G11" s="23"/>
       <c r="H11" s="13"/>
       <c r="I11" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J11" s="22"/>
       <c r="K11" s="22"/>
@@ -13376,7 +13373,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>20</v>
+        <v>101</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>15</v>
@@ -13391,68 +13388,68 @@
         <v>8</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J14" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="J14" s="4" t="s">
-        <v>28</v>
-      </c>
       <c r="K14" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M14" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N14" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="N14" s="6" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C15" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D15" s="6" t="s">
-        <v>77</v>
-      </c>
       <c r="E15" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>8</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J15" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="J15" s="4" t="s">
-        <v>28</v>
-      </c>
       <c r="K15" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N15" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -18120,17 +18117,17 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>36</v>
-      </c>
-    </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -18140,12 +18137,12 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -18160,7 +18157,7 @@
       <c r="G11" s="23"/>
       <c r="H11" s="13"/>
       <c r="I11" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J11" s="22"/>
       <c r="K11" s="22"/>
@@ -18232,35 +18229,35 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C14" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D14" s="6" t="s">
-        <v>77</v>
-      </c>
       <c r="E14" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>8</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L14" s="7"/>
       <c r="M14" s="4"/>
@@ -22949,17 +22946,17 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -22969,17 +22966,17 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -23088,7 +23085,7 @@
         <v>0</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>6</v>
@@ -23103,17 +23100,17 @@
         <v>8</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L15" s="7"/>
       <c r="M15" s="4"/>
@@ -23122,7 +23119,7 @@
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>6</v>
@@ -23137,17 +23134,17 @@
         <v>8</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H16" s="5"/>
       <c r="I16" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L16" s="7"/>
       <c r="M16" s="4"/>
@@ -23155,35 +23152,35 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C17" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D17" s="6" t="s">
-        <v>77</v>
-      </c>
       <c r="E17" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>8</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H17" s="5"/>
       <c r="I17" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L17" s="7"/>
       <c r="M17" s="4"/>
@@ -23192,32 +23189,32 @@
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="E18" s="7" t="s">
         <v>75</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>77</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>8</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L18" s="7"/>
       <c r="M18" s="4"/>
@@ -27769,7 +27766,7 @@
   <dimension ref="A1:O544"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27788,17 +27785,17 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -27808,17 +27805,17 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -27832,7 +27829,7 @@
       <c r="F11" s="22"/>
       <c r="G11" s="23"/>
       <c r="I11" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J11" s="22"/>
       <c r="K11" s="22"/>
@@ -27910,7 +27907,7 @@
         <v>0</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>6</v>
@@ -27925,17 +27922,17 @@
         <v>8</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J14" s="4" t="s">
         <v>10</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L14" s="7"/>
       <c r="M14" s="4"/>
@@ -27946,7 +27943,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>20</v>
+        <v>101</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>15</v>
@@ -27961,17 +27958,17 @@
         <v>8</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J15" s="4" t="s">
         <v>10</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L15" s="7"/>
       <c r="M15" s="4"/>
@@ -27979,35 +27976,35 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C16" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D16" s="6" t="s">
-        <v>77</v>
-      </c>
       <c r="E16" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>8</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H16" s="5"/>
       <c r="I16" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>10</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L16" s="7"/>
       <c r="M16" s="4"/>
@@ -28016,35 +28013,35 @@
     </row>
     <row r="17" spans="1:15" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C17" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="D17" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="D17" s="18" t="s">
-        <v>77</v>
-      </c>
       <c r="E17" s="16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F17" s="17" t="s">
         <v>8</v>
       </c>
       <c r="G17" s="18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H17" s="15"/>
       <c r="I17" s="16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J17" s="17" t="s">
         <v>10</v>
       </c>
       <c r="K17" s="18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L17" s="16"/>
       <c r="M17" s="17"/>
@@ -35289,17 +35286,17 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -35309,22 +35306,22 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -35433,7 +35430,7 @@
         <v>0</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>6</v>
@@ -35448,17 +35445,17 @@
         <v>8</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L15" s="7"/>
       <c r="M15" s="4"/>
@@ -35466,35 +35463,35 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C16" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D16" s="6" t="s">
-        <v>77</v>
-      </c>
       <c r="E16" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>8</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H16" s="5"/>
       <c r="I16" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L16" s="7"/>
       <c r="M16" s="4"/>
@@ -40045,7 +40042,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O550"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -40065,32 +40062,32 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>101</v>
-      </c>
-    </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -40100,12 +40097,12 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -40119,7 +40116,7 @@
       <c r="F14" s="22"/>
       <c r="G14" s="23"/>
       <c r="I14" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J14" s="22"/>
       <c r="K14" s="22"/>
@@ -40194,10 +40191,10 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>13</v>
@@ -40212,17 +40209,17 @@
         <v>8</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H17" s="5"/>
       <c r="I17" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L17" s="7"/>
       <c r="M17" s="4"/>
@@ -40231,10 +40228,10 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>13</v>
@@ -40249,17 +40246,17 @@
         <v>8</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L18" s="7"/>
       <c r="M18" s="4"/>
@@ -40268,29 +40265,29 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="4"/>
       <c r="G19" s="6"/>
       <c r="H19" s="5"/>
       <c r="I19" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L19" s="7"/>
       <c r="M19" s="4"/>

</xml_diff>

<commit_message>
Updated XSL file of external datasets linking.
</commit_message>
<xml_diff>
--- a/aliada/aliada-links-discovery/src/main/resources/ALIADA_datasets_links.xlsx
+++ b/aliada/aliada-links-discovery/src/main/resources/ALIADA_datasets_links.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="19440" windowHeight="7170"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="19440" windowHeight="7170" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="DBpedia" sheetId="5" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="99">
   <si>
     <t>Actor</t>
   </si>
@@ -75,9 +75,6 @@
   </si>
   <si>
     <t>Place</t>
-  </si>
-  <si>
-    <t>gn:Feature</t>
   </si>
   <si>
     <t>PREFIX ecrm:   &lt;http://erlangen-crm.org/current/&gt;</t>
@@ -191,21 +188,6 @@
     <t>SPARQL endpoint: http://datos.bne.es/sparql</t>
   </si>
   <si>
-    <t>PREFIX ifla-frbr:   &lt;http://iflastandards.info/ns/fr/frbr/frbrer/&gt;</t>
-  </si>
-  <si>
-    <t>ifla-frbr:C1005</t>
-  </si>
-  <si>
-    <t>ifla-frbr:P3039</t>
-  </si>
-  <si>
-    <t>ifla-frbr:C1001</t>
-  </si>
-  <si>
-    <t>ifla-frbr:P3001</t>
-  </si>
-  <si>
     <t># Triples: 1.9 billion triples</t>
   </si>
   <si>
@@ -245,9 +227,6 @@
     <t>ecrm:P102_has_title</t>
   </si>
   <si>
-    <t>efrbroo:E35_Title</t>
-  </si>
-  <si>
     <t>ecrm:E35_Title</t>
   </si>
   <si>
@@ -273,15 +252,6 @@
   </si>
   <si>
     <t xml:space="preserve"> fb:type.object.type fb:film.film</t>
-  </si>
-  <si>
-    <t>PREFIX ifla-frad:   &lt;http://iflastandards.info/ns/fr/frad/&gt;</t>
-  </si>
-  <si>
-    <t>ifla-frad:P4031</t>
-  </si>
-  <si>
-    <t>ifla-frad:P4033</t>
   </si>
   <si>
     <t># Triples: 8816?????</t>
@@ -328,6 +298,27 @@
   <si>
     <t>ecrm:E19_Physical_Object</t>
   </si>
+  <si>
+    <t>geo:Feature</t>
+  </si>
+  <si>
+    <t>PREFIX bne:   &lt;http://datos.bne.es/def/&gt;</t>
+  </si>
+  <si>
+    <t>bne:C1005</t>
+  </si>
+  <si>
+    <t>bne:C1003</t>
+  </si>
+  <si>
+    <t>bne:P1004</t>
+  </si>
+  <si>
+    <t>bne:P5001</t>
+  </si>
+  <si>
+    <t>ecrm:E73_Information_Object</t>
+  </si>
 </sst>
 </file>
 
@@ -348,7 +339,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -366,16 +357,6 @@
         <fgColor theme="6" tint="0.39994506668294322"/>
         <bgColor indexed="64"/>
       </patternFill>
-    </fill>
-    <fill>
-      <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
-        <stop position="0">
-          <color theme="0"/>
-        </stop>
-        <stop position="1">
-          <color theme="5" tint="0.40000610370189521"/>
-        </stop>
-      </gradientFill>
     </fill>
   </fills>
   <borders count="15">
@@ -546,7 +527,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -564,12 +545,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -897,7 +872,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N535"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -919,37 +894,37 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -973,46 +948,46 @@
       <c r="H10" s="9"/>
     </row>
     <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="23"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="17"/>
       <c r="H11" s="13"/>
-      <c r="I11" s="21" t="s">
+      <c r="I11" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="J11" s="22"/>
-      <c r="K11" s="22"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="22"/>
-      <c r="N11" s="23"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="17"/>
     </row>
     <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="26" t="s">
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
       <c r="H12" s="5"/>
-      <c r="I12" s="26" t="s">
+      <c r="I12" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="J12" s="27"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="26" t="s">
+      <c r="J12" s="21"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="M12" s="27"/>
-      <c r="N12" s="28"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="22"/>
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
@@ -1058,7 +1033,7 @@
         <v>0</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>6</v>
@@ -1073,17 +1048,17 @@
         <v>8</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L14" s="7"/>
       <c r="M14" s="4"/>
@@ -1094,7 +1069,7 @@
         <v>17</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>13</v>
@@ -1109,17 +1084,17 @@
         <v>8</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L15" s="7"/>
       <c r="M15" s="4"/>
@@ -1130,7 +1105,7 @@
         <v>12</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>15</v>
@@ -1145,17 +1120,17 @@
         <v>8</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H16" s="5"/>
       <c r="I16" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>10</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L16" s="7"/>
       <c r="M16" s="4"/>
@@ -1163,35 +1138,35 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>8</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H17" s="5"/>
       <c r="I17" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J17" s="4" t="s">
         <v>10</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L17" s="7"/>
       <c r="M17" s="4"/>
@@ -5743,7 +5718,7 @@
   <dimension ref="A1:O546"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5762,81 +5737,81 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>48</v>
-      </c>
-    </row>
     <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="23"/>
-      <c r="I11" s="21" t="s">
-        <v>32</v>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="17"/>
+      <c r="I11" s="15" t="s">
+        <v>31</v>
       </c>
-      <c r="J11" s="22"/>
-      <c r="K11" s="22"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="22"/>
-      <c r="N11" s="23"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="17"/>
       <c r="O11" s="9"/>
     </row>
     <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="26" t="s">
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
       <c r="H12" s="5"/>
-      <c r="I12" s="26" t="s">
+      <c r="I12" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="J12" s="27"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="26" t="s">
+      <c r="J12" s="21"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="M12" s="27"/>
-      <c r="N12" s="28"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="22"/>
       <c r="O12" s="9"/>
     </row>
     <row r="13" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5884,26 +5859,26 @@
         <v>17</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="4"/>
       <c r="G14" s="6"/>
       <c r="H14" s="5"/>
       <c r="I14" s="7" t="s">
-        <v>18</v>
+        <v>92</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L14" s="7"/>
       <c r="M14" s="4"/>
@@ -5913,7 +5888,7 @@
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="7" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>13</v>
@@ -5928,17 +5903,17 @@
         <v>8</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="7" t="s">
-        <v>18</v>
+        <v>92</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L15" s="7"/>
       <c r="M15" s="4"/>
@@ -13230,7 +13205,7 @@
   <dimension ref="A1:N543"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13248,86 +13223,86 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>25</v>
-      </c>
-    </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>29</v>
-      </c>
-    </row>
     <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="23"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="17"/>
       <c r="H11" s="13"/>
-      <c r="I11" s="21" t="s">
-        <v>33</v>
+      <c r="I11" s="15" t="s">
+        <v>32</v>
       </c>
-      <c r="J11" s="22"/>
-      <c r="K11" s="22"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="22"/>
-      <c r="N11" s="23"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="17"/>
     </row>
     <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="26" t="s">
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
       <c r="H12" s="5"/>
-      <c r="I12" s="26" t="s">
+      <c r="I12" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="J12" s="27"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="26" t="s">
+      <c r="J12" s="21"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="M12" s="27"/>
-      <c r="N12" s="28"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="22"/>
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
@@ -13373,7 +13348,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>15</v>
@@ -13388,68 +13363,68 @@
         <v>8</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J14" s="4" t="s">
-        <v>27</v>
-      </c>
       <c r="K14" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N14" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="N14" s="6" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>8</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J15" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J15" s="4" t="s">
-        <v>27</v>
-      </c>
       <c r="K15" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N15" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -18117,76 +18092,76 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>35</v>
-      </c>
-    </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="23"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="17"/>
       <c r="H11" s="13"/>
-      <c r="I11" s="21" t="s">
-        <v>40</v>
+      <c r="I11" s="15" t="s">
+        <v>39</v>
       </c>
-      <c r="J11" s="22"/>
-      <c r="K11" s="22"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="22"/>
-      <c r="N11" s="23"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="17"/>
     </row>
     <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="26" t="s">
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
       <c r="H12" s="5"/>
-      <c r="I12" s="26" t="s">
+      <c r="I12" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="J12" s="27"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="26" t="s">
+      <c r="J12" s="21"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="M12" s="27"/>
-      <c r="N12" s="28"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="22"/>
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
@@ -18229,35 +18204,35 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>8</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L14" s="7"/>
       <c r="M14" s="4"/>
@@ -22924,8 +22899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N536"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView topLeftCell="D7" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22946,37 +22921,37 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -23000,46 +22975,46 @@
       <c r="H11" s="9"/>
     </row>
     <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="23"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="17"/>
       <c r="H12" s="13"/>
-      <c r="I12" s="21" t="s">
+      <c r="I12" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="J12" s="22"/>
-      <c r="K12" s="22"/>
-      <c r="L12" s="22"/>
-      <c r="M12" s="22"/>
-      <c r="N12" s="23"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="17"/>
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="26" t="s">
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
       <c r="H13" s="5"/>
-      <c r="I13" s="26" t="s">
+      <c r="I13" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="J13" s="27"/>
-      <c r="K13" s="28"/>
-      <c r="L13" s="26" t="s">
+      <c r="J13" s="21"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="M13" s="27"/>
-      <c r="N13" s="28"/>
+      <c r="M13" s="21"/>
+      <c r="N13" s="22"/>
     </row>
     <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
@@ -23085,7 +23060,7 @@
         <v>0</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>6</v>
@@ -23100,17 +23075,17 @@
         <v>8</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="7" t="s">
-        <v>57</v>
+        <v>94</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>58</v>
+        <v>10</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L15" s="7"/>
       <c r="M15" s="4"/>
@@ -23119,7 +23094,7 @@
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="7" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>6</v>
@@ -23134,17 +23109,17 @@
         <v>8</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H16" s="5"/>
       <c r="I16" s="7" t="s">
-        <v>57</v>
+        <v>94</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L16" s="7"/>
       <c r="M16" s="4"/>
@@ -23152,35 +23127,35 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>8</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H17" s="5"/>
       <c r="I17" s="7" t="s">
-        <v>59</v>
+        <v>95</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L17" s="7"/>
       <c r="M17" s="4"/>
@@ -23189,32 +23164,32 @@
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="7" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>8</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="7" t="s">
-        <v>59</v>
+        <v>95</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L18" s="7"/>
       <c r="M18" s="4"/>
@@ -27765,8 +27740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O544"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="F7" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27785,81 +27760,81 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="23"/>
-      <c r="I11" s="21" t="s">
-        <v>32</v>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="17"/>
+      <c r="I11" s="15" t="s">
+        <v>31</v>
       </c>
-      <c r="J11" s="22"/>
-      <c r="K11" s="22"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="22"/>
-      <c r="N11" s="23"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="17"/>
       <c r="O11" s="9"/>
     </row>
     <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="26" t="s">
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
       <c r="H12" s="5"/>
-      <c r="I12" s="26" t="s">
+      <c r="I12" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="J12" s="27"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="26" t="s">
+      <c r="J12" s="21"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="M12" s="27"/>
-      <c r="N12" s="28"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="22"/>
       <c r="O12" s="9"/>
     </row>
     <row r="13" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -27907,7 +27882,7 @@
         <v>0</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>6</v>
@@ -27922,17 +27897,17 @@
         <v>8</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="7" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="J14" s="4" t="s">
         <v>10</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L14" s="7"/>
       <c r="M14" s="4"/>
@@ -27943,7 +27918,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>15</v>
@@ -27958,17 +27933,17 @@
         <v>8</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="7" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="J15" s="4" t="s">
         <v>10</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L15" s="7"/>
       <c r="M15" s="4"/>
@@ -27976,77 +27951,77 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>8</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H16" s="5"/>
       <c r="I16" s="7" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>10</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L16" s="7"/>
       <c r="M16" s="4"/>
       <c r="N16" s="6"/>
       <c r="O16" s="9"/>
     </row>
-    <row r="17" spans="1:15" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="B17" s="16" t="s">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C17" s="17" t="s">
-        <v>73</v>
+      <c r="B17" s="7" t="s">
+        <v>98</v>
       </c>
-      <c r="D17" s="18" t="s">
-        <v>75</v>
+      <c r="C17" s="4" t="s">
+        <v>67</v>
       </c>
-      <c r="E17" s="16" t="s">
-        <v>75</v>
+      <c r="D17" s="6" t="s">
+        <v>68</v>
       </c>
-      <c r="F17" s="17" t="s">
+      <c r="E17" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F17" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G17" s="18" t="s">
-        <v>52</v>
+      <c r="G17" s="6" t="s">
+        <v>51</v>
       </c>
-      <c r="H17" s="15"/>
-      <c r="I17" s="16" t="s">
-        <v>83</v>
+      <c r="H17" s="5"/>
+      <c r="I17" s="7" t="s">
+        <v>76</v>
       </c>
-      <c r="J17" s="17" t="s">
+      <c r="J17" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K17" s="18" t="s">
-        <v>52</v>
+      <c r="K17" s="6" t="s">
+        <v>51</v>
       </c>
-      <c r="L17" s="16"/>
-      <c r="M17" s="17"/>
-      <c r="N17" s="18"/>
-      <c r="O17" s="19"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="9"/>
     </row>
     <row r="18" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
@@ -35264,7 +35239,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N534"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="G4" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -35286,42 +35261,42 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>71</v>
-      </c>
-    </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -35345,46 +35320,46 @@
       <c r="H11" s="9"/>
     </row>
     <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="23"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="17"/>
       <c r="H12" s="13"/>
-      <c r="I12" s="21" t="s">
+      <c r="I12" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="J12" s="22"/>
-      <c r="K12" s="22"/>
-      <c r="L12" s="22"/>
-      <c r="M12" s="22"/>
-      <c r="N12" s="23"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="17"/>
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="26" t="s">
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
       <c r="H13" s="5"/>
-      <c r="I13" s="26" t="s">
+      <c r="I13" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="J13" s="27"/>
-      <c r="K13" s="28"/>
-      <c r="L13" s="26" t="s">
+      <c r="J13" s="21"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="M13" s="27"/>
-      <c r="N13" s="28"/>
+      <c r="M13" s="21"/>
+      <c r="N13" s="22"/>
     </row>
     <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
@@ -35430,7 +35405,7 @@
         <v>0</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>6</v>
@@ -35445,17 +35420,17 @@
         <v>8</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="7" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L15" s="7"/>
       <c r="M15" s="4"/>
@@ -35463,35 +35438,35 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>8</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H16" s="5"/>
       <c r="I16" s="7" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L16" s="7"/>
       <c r="M16" s="4"/>
@@ -40042,7 +40017,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O550"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="J10" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -40062,91 +40037,91 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="23"/>
-      <c r="I14" s="21" t="s">
-        <v>32</v>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="17"/>
+      <c r="I14" s="15" t="s">
+        <v>31</v>
       </c>
-      <c r="J14" s="22"/>
-      <c r="K14" s="22"/>
-      <c r="L14" s="22"/>
-      <c r="M14" s="22"/>
-      <c r="N14" s="23"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="16"/>
+      <c r="N14" s="17"/>
       <c r="O14" s="9"/>
     </row>
     <row r="15" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="26" t="s">
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
       <c r="H15" s="5"/>
-      <c r="I15" s="26" t="s">
+      <c r="I15" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="J15" s="27"/>
-      <c r="K15" s="28"/>
-      <c r="L15" s="26" t="s">
+      <c r="J15" s="21"/>
+      <c r="K15" s="22"/>
+      <c r="L15" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="M15" s="27"/>
-      <c r="N15" s="28"/>
+      <c r="M15" s="21"/>
+      <c r="N15" s="22"/>
       <c r="O15" s="9"/>
     </row>
     <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -40191,10 +40166,10 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>13</v>
@@ -40209,17 +40184,17 @@
         <v>8</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H17" s="5"/>
       <c r="I17" s="4" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L17" s="7"/>
       <c r="M17" s="4"/>
@@ -40228,10 +40203,10 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>13</v>
@@ -40246,17 +40221,17 @@
         <v>8</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="4" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L18" s="7"/>
       <c r="M18" s="4"/>
@@ -40265,29 +40240,29 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="4"/>
       <c r="G19" s="6"/>
       <c r="H19" s="5"/>
       <c r="I19" s="4" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L19" s="7"/>
       <c r="M19" s="4"/>

</xml_diff>

<commit_message>
Update linking configuration files.
</commit_message>
<xml_diff>
--- a/aliada/aliada-links-discovery/src/main/resources/ALIADA_datasets_links.xlsx
+++ b/aliada/aliada-links-discovery/src/main/resources/ALIADA_datasets_links.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="19440" windowHeight="7170" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="19440" windowHeight="7170"/>
   </bookViews>
   <sheets>
     <sheet name="DBpedia" sheetId="5" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="99">
   <si>
     <t>Actor</t>
   </si>
@@ -296,9 +296,6 @@
     <t>graph: http://id.loc.gov/vocabulary/geographicAreas</t>
   </si>
   <si>
-    <t>ecrm:E19_Physical_Object</t>
-  </si>
-  <si>
     <t>geo:Feature</t>
   </si>
   <si>
@@ -318,6 +315,9 @@
   </si>
   <si>
     <t>ecrm:E73_Information_Object</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ecrm:E18_Physical_Thing </t>
   </si>
 </sst>
 </file>
@@ -872,8 +872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N535"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18:K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1105,7 +1105,7 @@
         <v>12</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>15</v>
@@ -1173,17 +1173,37 @@
       <c r="N17" s="6"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="6"/>
+      <c r="A18" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>51</v>
+      </c>
       <c r="H18" s="5"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="6"/>
+      <c r="I18" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K18" s="6" t="s">
+        <v>51</v>
+      </c>
       <c r="L18" s="7"/>
       <c r="M18" s="4"/>
       <c r="N18" s="6"/>
@@ -5872,7 +5892,7 @@
       <c r="G14" s="6"/>
       <c r="H14" s="5"/>
       <c r="I14" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J14" s="4" t="s">
         <v>48</v>
@@ -5907,7 +5927,7 @@
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J15" s="4" t="s">
         <v>49</v>
@@ -13204,8 +13224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N543"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16:N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13348,7 +13368,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>15</v>
@@ -13428,20 +13448,46 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="6"/>
+      <c r="A16" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>51</v>
+      </c>
       <c r="H16" s="5"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="6"/>
+      <c r="I16" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="L16" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N16" s="6" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
@@ -22946,7 +22992,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -23079,7 +23125,7 @@
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J15" s="4" t="s">
         <v>10</v>
@@ -23113,10 +23159,10 @@
       </c>
       <c r="H16" s="5"/>
       <c r="I16" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K16" s="6" t="s">
         <v>51</v>
@@ -23149,7 +23195,7 @@
       </c>
       <c r="H17" s="5"/>
       <c r="I17" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J17" s="4" t="s">
         <v>10</v>
@@ -23183,10 +23229,10 @@
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K18" s="6" t="s">
         <v>51</v>
@@ -27740,8 +27786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O544"/>
   <sheetViews>
-    <sheetView topLeftCell="F7" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="D7" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27918,7 +27964,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>15</v>
@@ -27991,7 +28037,7 @@
         <v>72</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>67</v>
@@ -40017,7 +40063,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O550"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J10" workbookViewId="0">
+    <sheetView topLeftCell="J10" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>